<commit_message>
Include PWR_CCS in groups
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_CCS.xlsx
+++ b/SuppXLS/Scen_PWR_CCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018077B9-1987-43FF-B10C-C4A4131F2963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A665C7-4C41-4820-9C01-64C183956714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
   <si>
     <t>UC_N</t>
   </si>
@@ -470,9 +470,6 @@
   <si>
     <t>P-TH*CCS*</t>
     <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Allregions</t>
   </si>
   <si>
     <t>PWRCO2N</t>
@@ -702,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -758,6 +755,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2000,8 +1998,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,32 +2407,33 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0058FA53-D765-4D61-875F-79F603B8624E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="26"/>
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
-    </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
         <v>118</v>
       </c>
@@ -2447,110 +2446,131 @@
       <c r="E3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="F3" s="28" t="str">
+        <f>Regions!C3</f>
+        <v>IE</v>
+      </c>
+      <c r="G3" s="28" t="str">
+        <f>Regions!D3</f>
+        <v>National</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="I3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="J3" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="K3" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="L3" s="29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D4" s="30" t="s">
         <v>124</v>
       </c>
       <c r="F4" s="31">
         <v>6.7320000000000002</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>128</v>
+      <c r="G4" s="31">
+        <f t="shared" ref="G4:G9" si="0">F4</f>
+        <v>6.7320000000000002</v>
       </c>
       <c r="H4" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30" t="s">
-        <v>128</v>
-      </c>
+      <c r="J4" s="30"/>
       <c r="K4" s="30" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D5" s="32" t="s">
         <v>124</v>
       </c>
       <c r="F5" s="33">
         <v>49.368000000000002</v>
       </c>
-      <c r="G5" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="30" t="s">
+      <c r="G5" s="33">
+        <f t="shared" si="0"/>
+        <v>49.368000000000002</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32" t="s">
-        <v>128</v>
-      </c>
+      <c r="J5" s="32"/>
       <c r="K5" s="32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D6" s="30" t="s">
         <v>124</v>
       </c>
       <c r="F6" s="31">
         <v>11.795999999999999</v>
       </c>
-      <c r="G6" s="30" t="s">
-        <v>129</v>
+      <c r="G6" s="31">
+        <f t="shared" si="0"/>
+        <v>11.795999999999999</v>
       </c>
       <c r="H6" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30" t="s">
-        <v>129</v>
-      </c>
+      <c r="J6" s="30"/>
       <c r="K6" s="30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D7" s="30" t="s">
         <v>124</v>
       </c>
       <c r="F7" s="31">
         <v>12.144</v>
       </c>
-      <c r="G7" s="30" t="s">
-        <v>130</v>
+      <c r="G7" s="31">
+        <f t="shared" si="0"/>
+        <v>12.144</v>
       </c>
       <c r="H7" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30" t="s">
-        <v>130</v>
-      </c>
+      <c r="J7" s="30"/>
       <c r="K7" s="30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D8" s="32" t="s">
         <v>124</v>
       </c>
@@ -2558,21 +2578,25 @@
       <c r="F8" s="32">
         <v>87.204000000000008</v>
       </c>
-      <c r="G8" s="30" t="s">
-        <v>129</v>
+      <c r="G8" s="33">
+        <f t="shared" si="0"/>
+        <v>87.204000000000008</v>
       </c>
       <c r="H8" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="32"/>
+      <c r="K8" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="35" t="s">
@@ -2582,18 +2606,22 @@
       <c r="F9" s="35">
         <v>95.855999999999995</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="36">
+        <f t="shared" si="0"/>
+        <v>95.855999999999995</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="35"/>
+      <c r="K9" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" s="32" t="s">
         <v>130</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" s="35"/>
-      <c r="J9" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="K9" s="32" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2602,6 +2630,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2747,22 +2790,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5B0C690-3E0C-4B9D-864A-3F51F2CB2C74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04886123-9BA9-4DD3-969B-04E608718995}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA27B0CF-89B5-4B4C-B311-C0E79941CE35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2778,21 +2823,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04886123-9BA9-4DD3-969B-04E608718995}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5B0C690-3E0C-4B9D-864A-3F51F2CB2C74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Use FLO_EMIS instead of ENVACT with CCS and keep it only in Scen_PWR_CCS.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_CCS.xlsx
+++ b/SuppXLS/Scen_PWR_CCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A665C7-4C41-4820-9C01-64C183956714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C5AFC-FA2F-4ED4-94FD-15CE65137806}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
   <si>
     <t>UC_N</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>PWRCO2S</t>
+  </si>
+  <si>
+    <t>PWRBIO</t>
+  </si>
+  <si>
+    <t>P-*CCS*</t>
   </si>
 </sst>
 </file>
@@ -699,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -753,7 +759,6 @@
     <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -1998,8 +2003,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,10 +2412,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0058FA53-D765-4D61-875F-79F603B8624E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:L9"/>
+  <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,7 +2483,7 @@
         <v>6.7320000000000002</v>
       </c>
       <c r="G4" s="31">
-        <f t="shared" ref="G4:G9" si="0">F4</f>
+        <f t="shared" ref="G4:G8" si="0">F4</f>
         <v>6.7320000000000002</v>
       </c>
       <c r="H4" s="30" t="s">
@@ -2488,8 +2493,9 @@
         <v>125</v>
       </c>
       <c r="J4" s="30"/>
-      <c r="K4" s="30" t="s">
-        <v>127</v>
+      <c r="K4" s="30" t="str">
+        <f t="shared" ref="K4:K11" si="1">H4</f>
+        <v>PWRGAS</v>
       </c>
       <c r="L4" s="30" t="s">
         <v>126</v>
@@ -2513,8 +2519,9 @@
         <v>125</v>
       </c>
       <c r="J5" s="32"/>
-      <c r="K5" s="32" t="s">
-        <v>127</v>
+      <c r="K5" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>PWRGAS</v>
       </c>
       <c r="L5" s="32" t="s">
         <v>130</v>
@@ -2538,76 +2545,77 @@
         <v>125</v>
       </c>
       <c r="J6" s="30"/>
-      <c r="K6" s="30" t="s">
-        <v>128</v>
+      <c r="K6" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v>PWRCOA</v>
       </c>
       <c r="L6" s="30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D7" s="30" t="s">
+    <row r="7" spans="2:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="31">
+      <c r="E7" s="32"/>
+      <c r="F7" s="32">
+        <v>87.204000000000008</v>
+      </c>
+      <c r="G7" s="33">
+        <f>F7</f>
+        <v>87.204000000000008</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="30" t="str">
+        <f>H7</f>
+        <v>PWRCOA</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="31">
         <v>12.144</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G8" s="31">
         <f t="shared" si="0"/>
         <v>12.144</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H8" s="30" t="s">
         <v>129</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="L7" s="30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32">
-        <v>87.204000000000008</v>
-      </c>
-      <c r="G8" s="33">
-        <f t="shared" si="0"/>
-        <v>87.204000000000008</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>128</v>
       </c>
       <c r="I8" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="L8" s="32" t="s">
-        <v>130</v>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v>PWRPEA</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35">
+      <c r="E9" s="34"/>
+      <c r="F9" s="34">
         <v>95.855999999999995</v>
       </c>
-      <c r="G9" s="36">
-        <f t="shared" si="0"/>
+      <c r="G9" s="35">
+        <f>F9</f>
         <v>95.855999999999995</v>
       </c>
       <c r="H9" s="30" t="s">
@@ -2616,11 +2624,66 @@
       <c r="I9" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="30" t="s">
-        <v>129</v>
+      <c r="J9" s="34"/>
+      <c r="K9" s="30" t="str">
+        <f>H9</f>
+        <v>PWRPEA</v>
       </c>
       <c r="L9" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32">
+        <v>-79.73</v>
+      </c>
+      <c r="G10" s="33">
+        <f t="shared" ref="G10:G11" si="2">F10</f>
+        <v>-79.73</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v>PWRBIO</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34">
+        <v>79.73</v>
+      </c>
+      <c r="G11" s="35">
+        <f t="shared" si="2"/>
+        <v>79.73</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="J11" s="34"/>
+      <c r="K11" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v>PWRBIO</v>
+      </c>
+      <c r="L11" s="32" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2630,21 +2693,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2790,24 +2838,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5B0C690-3E0C-4B9D-864A-3F51F2CB2C74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04886123-9BA9-4DD3-969B-04E608718995}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA27B0CF-89B5-4B4C-B311-C0E79941CE35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2823,4 +2869,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04886123-9BA9-4DD3-969B-04E608718995}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5B0C690-3E0C-4B9D-864A-3F51F2CB2C74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>